<commit_message>
added some TITN 10-K notes
</commit_message>
<xml_diff>
--- a/CNH/CNH.xlsx
+++ b/CNH/CNH.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/32906c935fa0eb4f/models/CNH/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1087" documentId="11_F25DC773A252ABDACC104889191A52245ADE58E6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{94F0F81C-EADC-49AD-86EF-DA93301142D2}"/>
+  <xr:revisionPtr revIDLastSave="1096" documentId="11_F25DC773A252ABDACC104889191A52245ADE58E6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B924C7EE-2C81-4696-BFE6-8A920000A929}"/>
   <bookViews>
-    <workbookView xWindow="18730" yWindow="3990" windowWidth="17190" windowHeight="15850" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22750" yWindow="4020" windowWidth="15080" windowHeight="15850" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="2" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="149">
   <si>
     <t>Revenues</t>
   </si>
@@ -475,6 +475,18 @@
   </si>
   <si>
     <t>De-merged from Iveco Group - starting Q122</t>
+  </si>
+  <si>
+    <t>Purchased Specialty Enterprises, LLC, manufacturer of spray booms and spray boom accessories. $50M.</t>
+  </si>
+  <si>
+    <t>Q421</t>
+  </si>
+  <si>
+    <t>Purchased 90% of Sampierana S.p.A. for $100M. Italian company specializing in the development, manufacture, and commercialization of earthmoving machines, undercarriages, and spare parts.</t>
+  </si>
+  <si>
+    <t>Purchased 100% of cap stock of Raven Industries, Inc. - total $2.1B. Based in Sioux Falls, SD. 3 business divisions: Applied Tech (precision ag tech), Engineered Films, and Aerostar. Engineered Films and Aerostar were held for sale.</t>
   </si>
 </sst>
 </file>
@@ -527,19 +539,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1027,15 +1037,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N105"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E6" sqref="E6"/>
+      <selection pane="topRight" activeCell="F76" sqref="F76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="31.7265625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="0" style="8" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="0" style="6" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
@@ -1066,7 +1076,7 @@
       <c r="K1" s="1">
         <v>2022</v>
       </c>
-      <c r="L1" s="8">
+      <c r="L1" s="6">
         <v>2023</v>
       </c>
       <c r="M1" s="1">
@@ -1104,10 +1114,10 @@
       </c>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
-      <c r="K2" s="6">
+      <c r="K2" s="3">
         <v>17969</v>
       </c>
-      <c r="L2" s="9">
+      <c r="L2" s="7">
         <v>18148</v>
       </c>
       <c r="M2" s="3">
@@ -1147,10 +1157,10 @@
       </c>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
-      <c r="K3" s="6">
+      <c r="K3" s="3">
         <v>3572</v>
       </c>
-      <c r="L3" s="9">
+      <c r="L3" s="7">
         <v>3932</v>
       </c>
       <c r="M3" s="3">
@@ -1203,7 +1213,7 @@
         <f t="shared" si="3"/>
         <v>21541</v>
       </c>
-      <c r="L4" s="10">
+      <c r="L4" s="8">
         <f t="shared" si="3"/>
         <v>22080</v>
       </c>
@@ -1244,10 +1254,10 @@
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
-      <c r="K5" s="6">
+      <c r="K5" s="3">
         <v>1996</v>
       </c>
-      <c r="L5" s="9">
+      <c r="L5" s="7">
         <v>2573</v>
       </c>
       <c r="M5" s="3">
@@ -1287,10 +1297,10 @@
       </c>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
-      <c r="K6" s="6">
+      <c r="K6" s="3">
         <v>14</v>
       </c>
-      <c r="L6" s="9">
+      <c r="L6" s="7">
         <v>34</v>
       </c>
       <c r="M6" s="3">
@@ -1343,7 +1353,7 @@
         <f t="shared" si="7"/>
         <v>23551</v>
       </c>
-      <c r="L7" s="10">
+      <c r="L7" s="8">
         <f t="shared" si="7"/>
         <v>24687</v>
       </c>
@@ -1366,8 +1376,8 @@
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="9"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="7"/>
       <c r="M8" s="4"/>
       <c r="N8" s="4"/>
     </row>
@@ -1384,8 +1394,8 @@
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
-      <c r="K9" s="6"/>
-      <c r="L9" s="9"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="7"/>
       <c r="M9" s="4"/>
       <c r="N9" s="4"/>
     </row>
@@ -1417,10 +1427,10 @@
       </c>
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
-      <c r="K10" s="6">
+      <c r="K10" s="3">
         <v>6769</v>
       </c>
-      <c r="L10" s="9">
+      <c r="L10" s="7">
         <v>7157</v>
       </c>
       <c r="M10" s="3">
@@ -1460,10 +1470,10 @@
       </c>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
-      <c r="K11" s="6">
+      <c r="K11" s="3">
         <v>5776</v>
       </c>
-      <c r="L11" s="9">
+      <c r="L11" s="7">
         <v>5878</v>
       </c>
       <c r="M11" s="3">
@@ -1503,10 +1513,10 @@
       </c>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
-      <c r="K12" s="6">
+      <c r="K12" s="3">
         <v>3738</v>
       </c>
-      <c r="L12" s="9">
+      <c r="L12" s="7">
         <v>3178</v>
       </c>
       <c r="M12" s="3">
@@ -1546,10 +1556,10 @@
       </c>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
-      <c r="K13" s="6">
+      <c r="K13" s="3">
         <v>1686</v>
       </c>
-      <c r="L13" s="9">
+      <c r="L13" s="7">
         <v>1935</v>
       </c>
       <c r="M13" s="3">
@@ -1602,7 +1612,7 @@
         <f t="shared" ref="K14:N14" si="12">SUM(K10:K13)</f>
         <v>17969</v>
       </c>
-      <c r="L14" s="10">
+      <c r="L14" s="8">
         <f t="shared" si="12"/>
         <v>18148</v>
       </c>
@@ -1625,8 +1635,8 @@
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
       <c r="J15" s="4"/>
-      <c r="K15" s="6"/>
-      <c r="L15" s="9"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="7"/>
       <c r="M15" s="3"/>
       <c r="N15" s="4"/>
     </row>
@@ -1655,8 +1665,8 @@
       </c>
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
-      <c r="K16" s="6"/>
-      <c r="L16" s="9"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="7"/>
       <c r="M16" s="3">
         <f>SUM(B16:E16)</f>
         <v>16031</v>
@@ -1691,8 +1701,8 @@
       </c>
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
-      <c r="K17" s="6"/>
-      <c r="L17" s="9"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="7"/>
       <c r="M17" s="3">
         <f>SUM(B17:E17)</f>
         <v>31</v>
@@ -1743,7 +1753,7 @@
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="L18" s="10">
+      <c r="L18" s="8">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
@@ -1781,8 +1791,8 @@
       </c>
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
-      <c r="K19" s="6"/>
-      <c r="L19" s="9"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="7"/>
       <c r="M19" s="3">
         <f>SUM(B19:E19)</f>
         <v>1342</v>
@@ -1817,8 +1827,8 @@
       </c>
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
-      <c r="K20" s="6"/>
-      <c r="L20" s="9"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="7"/>
       <c r="M20" s="3">
         <f>SUM(B20:E20)</f>
         <v>491</v>
@@ -1869,7 +1879,7 @@
         <f t="shared" si="18"/>
         <v>0</v>
       </c>
-      <c r="L21" s="10">
+      <c r="L21" s="8">
         <f t="shared" si="18"/>
         <v>0</v>
       </c>
@@ -1883,15 +1893,15 @@
       </c>
     </row>
     <row r="22" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="K22" s="7"/>
-      <c r="L22" s="11"/>
+      <c r="K22"/>
+      <c r="L22" s="9"/>
     </row>
     <row r="23" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="K23" s="7"/>
-      <c r="L23" s="11"/>
+      <c r="K23"/>
+      <c r="L23" s="9"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
@@ -1921,10 +1931,10 @@
       </c>
       <c r="I24" s="3"/>
       <c r="J24" s="3"/>
-      <c r="K24" s="6">
+      <c r="K24" s="3">
         <v>21541</v>
       </c>
-      <c r="L24" s="9">
+      <c r="L24" s="7">
         <v>22080</v>
       </c>
       <c r="M24" s="3">
@@ -1964,10 +1974,10 @@
       </c>
       <c r="I25" s="3"/>
       <c r="J25" s="3"/>
-      <c r="K25" s="6">
+      <c r="K25" s="3">
         <v>2010</v>
       </c>
-      <c r="L25" s="9">
+      <c r="L25" s="7">
         <v>2607</v>
       </c>
       <c r="M25" s="3">
@@ -2020,7 +2030,7 @@
         <f t="shared" ref="K26" si="21">SUM(K24:K25)</f>
         <v>23551</v>
       </c>
-      <c r="L26" s="10">
+      <c r="L26" s="8">
         <f t="shared" si="20"/>
         <v>24687</v>
       </c>
@@ -2061,10 +2071,10 @@
       </c>
       <c r="I27" s="3"/>
       <c r="J27" s="3"/>
-      <c r="K27" s="6">
+      <c r="K27" s="3">
         <v>16797</v>
       </c>
-      <c r="L27" s="9">
+      <c r="L27" s="7">
         <v>16838</v>
       </c>
       <c r="M27" s="3">
@@ -2117,7 +2127,7 @@
         <f t="shared" ref="K28" si="24">K26-K27</f>
         <v>6754</v>
       </c>
-      <c r="L28" s="10">
+      <c r="L28" s="8">
         <f t="shared" si="23"/>
         <v>7849</v>
       </c>
@@ -2158,10 +2168,10 @@
       </c>
       <c r="I29" s="3"/>
       <c r="J29" s="3"/>
-      <c r="K29" s="6">
+      <c r="K29" s="3">
         <v>1752</v>
       </c>
-      <c r="L29" s="9">
+      <c r="L29" s="7">
         <v>1863</v>
       </c>
       <c r="M29" s="3">
@@ -2201,10 +2211,10 @@
       </c>
       <c r="I30" s="3"/>
       <c r="J30" s="3"/>
-      <c r="K30" s="6">
+      <c r="K30" s="3">
         <v>866</v>
       </c>
-      <c r="L30" s="9">
+      <c r="L30" s="7">
         <v>1041</v>
       </c>
       <c r="M30" s="3">
@@ -2244,10 +2254,10 @@
       </c>
       <c r="I31" s="3"/>
       <c r="J31" s="3"/>
-      <c r="K31" s="6">
+      <c r="K31" s="3">
         <v>31</v>
       </c>
-      <c r="L31" s="9">
+      <c r="L31" s="7">
         <v>67</v>
       </c>
       <c r="M31" s="3">
@@ -2287,10 +2297,10 @@
       </c>
       <c r="I32" s="3"/>
       <c r="J32" s="3"/>
-      <c r="K32" s="6">
+      <c r="K32" s="3">
         <v>734</v>
       </c>
-      <c r="L32" s="9">
+      <c r="L32" s="7">
         <v>1345</v>
       </c>
       <c r="M32" s="3">
@@ -2330,10 +2340,10 @@
       </c>
       <c r="I33" s="3"/>
       <c r="J33" s="3"/>
-      <c r="K33" s="6">
+      <c r="K33" s="3">
         <v>689</v>
       </c>
-      <c r="L33" s="9">
+      <c r="L33" s="7">
         <v>830</v>
       </c>
       <c r="M33" s="3">
@@ -2386,7 +2396,7 @@
         <f t="shared" ref="K34:L34" si="29">SUM(K29:K33)+K27</f>
         <v>20869</v>
       </c>
-      <c r="L34" s="10">
+      <c r="L34" s="8">
         <f t="shared" si="29"/>
         <v>21984</v>
       </c>
@@ -2440,7 +2450,7 @@
         <f t="shared" ref="K35:L35" si="33">K26-K34</f>
         <v>2682</v>
       </c>
-      <c r="L35" s="10">
+      <c r="L35" s="8">
         <f t="shared" si="33"/>
         <v>2703</v>
       </c>
@@ -2481,10 +2491,10 @@
       </c>
       <c r="I36" s="3"/>
       <c r="J36" s="3"/>
-      <c r="K36" s="6">
+      <c r="K36" s="3">
         <v>-747</v>
       </c>
-      <c r="L36" s="9">
+      <c r="L36" s="7">
         <v>-594</v>
       </c>
       <c r="M36" s="3">
@@ -2524,10 +2534,10 @@
       </c>
       <c r="I37" s="3"/>
       <c r="J37" s="3"/>
-      <c r="K37" s="6">
+      <c r="K37" s="3">
         <v>104</v>
       </c>
-      <c r="L37" s="9">
+      <c r="L37" s="7">
         <v>274</v>
       </c>
       <c r="M37" s="3">
@@ -2567,10 +2577,10 @@
       </c>
       <c r="I38" s="3"/>
       <c r="J38" s="3"/>
-      <c r="K38" s="6">
+      <c r="K38" s="3">
         <v>10</v>
       </c>
-      <c r="L38" s="9">
+      <c r="L38" s="7">
         <v>12</v>
       </c>
       <c r="M38" s="3">
@@ -2623,7 +2633,7 @@
         <f t="shared" ref="K39" si="37">K35+K36+K37-K38</f>
         <v>2029</v>
       </c>
-      <c r="L39" s="10">
+      <c r="L39" s="8">
         <f t="shared" si="36"/>
         <v>2371</v>
       </c>
@@ -2637,8 +2647,7 @@
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="K40" s="7"/>
-      <c r="L40" s="11"/>
+      <c r="L40" s="9"/>
     </row>
     <row r="41" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
@@ -2681,7 +2690,7 @@
         <f t="shared" ref="K41:L41" si="40">K39/K44</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="L41" s="12" t="e">
+      <c r="L41" s="10" t="e">
         <f t="shared" si="40"/>
         <v>#DIV/0!</v>
       </c>
@@ -2735,7 +2744,7 @@
         <f t="shared" ref="K42:L42" si="43">K39/K45</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="L42" s="12" t="e">
+      <c r="L42" s="10" t="e">
         <f t="shared" si="43"/>
         <v>#DIV/0!</v>
       </c>
@@ -2749,8 +2758,7 @@
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="K43" s="7"/>
-      <c r="L43" s="11"/>
+      <c r="L43" s="9"/>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
@@ -2774,8 +2782,7 @@
       <c r="H44">
         <v>1332</v>
       </c>
-      <c r="K44" s="7"/>
-      <c r="L44" s="11"/>
+      <c r="L44" s="9"/>
       <c r="M44">
         <f>SUM(B44:E44)</f>
         <v>3934</v>
@@ -2807,8 +2814,7 @@
       <c r="H45">
         <v>1351</v>
       </c>
-      <c r="K45" s="7"/>
-      <c r="L45" s="11"/>
+      <c r="L45" s="9"/>
       <c r="M45">
         <f>SUM(B45:E45)</f>
         <v>3968</v>
@@ -2819,8 +2825,7 @@
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="K46" s="7"/>
-      <c r="L46" s="11"/>
+      <c r="L46" s="9"/>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
@@ -2838,8 +2843,7 @@
       <c r="H47">
         <v>0</v>
       </c>
-      <c r="K47" s="7"/>
-      <c r="L47" s="11"/>
+      <c r="L47" s="9"/>
       <c r="M47">
         <f>SUM(B47:E47)</f>
         <v>0</v>
@@ -2850,8 +2854,7 @@
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="K48" s="7"/>
-      <c r="L48" s="11"/>
+      <c r="L48" s="9"/>
     </row>
     <row r="49" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B49" s="1" t="str">
@@ -2886,8 +2889,8 @@
         <f t="shared" si="44"/>
         <v>Q424</v>
       </c>
-      <c r="K49" s="7"/>
-      <c r="L49" s="11"/>
+      <c r="K49"/>
+      <c r="L49" s="9"/>
       <c r="M49" s="1">
         <f t="shared" si="44"/>
         <v>2023</v>
@@ -2898,8 +2901,7 @@
       </c>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="K50" s="7"/>
-      <c r="L50" s="11"/>
+      <c r="L50" s="9"/>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
@@ -2933,8 +2935,8 @@
       </c>
       <c r="I51" s="3"/>
       <c r="J51" s="3"/>
-      <c r="K51" s="6"/>
-      <c r="L51" s="9">
+      <c r="K51" s="3"/>
+      <c r="L51" s="7">
         <v>2383</v>
       </c>
       <c r="M51" s="3">
@@ -2978,8 +2980,8 @@
       </c>
       <c r="I52" s="3"/>
       <c r="J52" s="3"/>
-      <c r="K52" s="6"/>
-      <c r="L52" s="9">
+      <c r="K52" s="3"/>
+      <c r="L52" s="7">
         <v>377</v>
       </c>
       <c r="M52" s="3">
@@ -3023,8 +3025,8 @@
       </c>
       <c r="I53" s="3"/>
       <c r="J53" s="3"/>
-      <c r="K53" s="6"/>
-      <c r="L53" s="9">
+      <c r="K53" s="3"/>
+      <c r="L53" s="7">
         <v>187</v>
       </c>
       <c r="M53" s="3">
@@ -3068,8 +3070,8 @@
       </c>
       <c r="I54" s="3"/>
       <c r="J54" s="3"/>
-      <c r="K54" s="6"/>
-      <c r="L54" s="9">
+      <c r="K54" s="3"/>
+      <c r="L54" s="7">
         <v>10</v>
       </c>
       <c r="M54" s="3">
@@ -3113,8 +3115,8 @@
       </c>
       <c r="I55" s="3"/>
       <c r="J55" s="3"/>
-      <c r="K55" s="6"/>
-      <c r="L55" s="9">
+      <c r="K55" s="3"/>
+      <c r="L55" s="7">
         <v>-211</v>
       </c>
       <c r="M55" s="3">
@@ -3158,8 +3160,8 @@
       </c>
       <c r="I56" s="3"/>
       <c r="J56" s="3"/>
-      <c r="K56" s="6"/>
-      <c r="L56" s="9">
+      <c r="K56" s="3"/>
+      <c r="L56" s="7">
         <v>173</v>
       </c>
       <c r="M56" s="3">
@@ -3203,8 +3205,8 @@
       </c>
       <c r="I57" s="3"/>
       <c r="J57" s="3"/>
-      <c r="K57" s="6"/>
-      <c r="L57" s="9">
+      <c r="K57" s="3"/>
+      <c r="L57" s="7">
         <v>911</v>
       </c>
       <c r="M57" s="3">
@@ -3248,8 +3250,8 @@
       </c>
       <c r="I58" s="3"/>
       <c r="J58" s="3"/>
-      <c r="K58" s="6"/>
-      <c r="L58" s="9">
+      <c r="K58" s="3"/>
+      <c r="L58" s="7">
         <v>-535</v>
       </c>
       <c r="M58" s="3">
@@ -3293,8 +3295,8 @@
       </c>
       <c r="I59" s="3"/>
       <c r="J59" s="3"/>
-      <c r="K59" s="6"/>
-      <c r="L59" s="9">
+      <c r="K59" s="3"/>
+      <c r="L59" s="7">
         <v>-2268</v>
       </c>
       <c r="M59" s="3">
@@ -3338,8 +3340,8 @@
       </c>
       <c r="I60" s="3"/>
       <c r="J60" s="3"/>
-      <c r="K60" s="6"/>
-      <c r="L60" s="9">
+      <c r="K60" s="3"/>
+      <c r="L60" s="7">
         <v>-259</v>
       </c>
       <c r="M60" s="3">
@@ -3383,8 +3385,8 @@
       </c>
       <c r="I61" s="3"/>
       <c r="J61" s="3"/>
-      <c r="K61" s="6"/>
-      <c r="L61" s="9">
+      <c r="K61" s="3"/>
+      <c r="L61" s="7">
         <v>-157</v>
       </c>
       <c r="M61" s="3">
@@ -3428,8 +3430,8 @@
       </c>
       <c r="I62" s="3"/>
       <c r="J62" s="3"/>
-      <c r="K62" s="6"/>
-      <c r="L62" s="9">
+      <c r="K62" s="3"/>
+      <c r="L62" s="7">
         <v>296</v>
       </c>
       <c r="M62" s="3">
@@ -3478,8 +3480,8 @@
         <v>0</v>
       </c>
       <c r="J63" s="4"/>
-      <c r="K63" s="6"/>
-      <c r="L63" s="10">
+      <c r="K63" s="3"/>
+      <c r="L63" s="8">
         <f t="shared" si="49"/>
         <v>907</v>
       </c>
@@ -3493,8 +3495,7 @@
       </c>
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="K64" s="7"/>
-      <c r="L64" s="11"/>
+      <c r="L64" s="9"/>
     </row>
     <row r="65" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B65" s="1" t="str">
@@ -3529,8 +3530,8 @@
         <f t="shared" si="50"/>
         <v>Q424</v>
       </c>
-      <c r="K65" s="7"/>
-      <c r="L65" s="11"/>
+      <c r="K65"/>
+      <c r="L65" s="9"/>
       <c r="M65" s="1">
         <f t="shared" si="50"/>
         <v>2023</v>
@@ -3541,15 +3542,14 @@
       </c>
     </row>
     <row r="66" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="K66" s="7"/>
-      <c r="L66" s="11"/>
+      <c r="L66" s="9"/>
     </row>
     <row r="67" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="K67" s="7"/>
-      <c r="L67" s="11"/>
+      <c r="K67"/>
+      <c r="L67" s="9"/>
     </row>
     <row r="68" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
@@ -3578,8 +3578,7 @@
       </c>
       <c r="I68" s="3"/>
       <c r="J68" s="3"/>
-      <c r="K68" s="7"/>
-      <c r="L68" s="11"/>
+      <c r="L68" s="9"/>
       <c r="M68" s="3">
         <f>E68</f>
         <v>4322</v>
@@ -3616,8 +3615,7 @@
       </c>
       <c r="I69" s="3"/>
       <c r="J69" s="3"/>
-      <c r="K69" s="7"/>
-      <c r="L69" s="11"/>
+      <c r="L69" s="9"/>
       <c r="M69" s="3">
         <f t="shared" ref="M69:M73" si="52">E69</f>
         <v>133</v>
@@ -3654,8 +3652,7 @@
       </c>
       <c r="I70" s="3"/>
       <c r="J70" s="3"/>
-      <c r="K70" s="7"/>
-      <c r="L70" s="11"/>
+      <c r="L70" s="9"/>
       <c r="M70" s="3">
         <f t="shared" si="52"/>
         <v>24249</v>
@@ -3692,8 +3689,7 @@
       </c>
       <c r="I71" s="3"/>
       <c r="J71" s="3"/>
-      <c r="K71" s="7"/>
-      <c r="L71" s="11"/>
+      <c r="L71" s="9"/>
       <c r="M71" s="3">
         <f t="shared" si="52"/>
         <v>380</v>
@@ -3730,8 +3726,7 @@
       </c>
       <c r="I72" s="3"/>
       <c r="J72" s="3"/>
-      <c r="K72" s="7"/>
-      <c r="L72" s="11"/>
+      <c r="L72" s="9"/>
       <c r="M72" s="3">
         <f t="shared" si="52"/>
         <v>5545</v>
@@ -3768,8 +3763,7 @@
       </c>
       <c r="I73" s="3"/>
       <c r="J73" s="3"/>
-      <c r="K73" s="7"/>
-      <c r="L73" s="11"/>
+      <c r="L73" s="9"/>
       <c r="M73" s="3">
         <f t="shared" si="52"/>
         <v>1417</v>
@@ -3816,8 +3810,8 @@
         <v>0</v>
       </c>
       <c r="J74" s="4"/>
-      <c r="K74" s="6"/>
-      <c r="L74" s="9"/>
+      <c r="K74" s="3"/>
+      <c r="L74" s="7"/>
       <c r="M74" s="4">
         <f>SUM(M68:M73)</f>
         <v>36046</v>
@@ -3854,8 +3848,7 @@
       </c>
       <c r="I75" s="3"/>
       <c r="J75" s="3"/>
-      <c r="K75" s="7"/>
-      <c r="L75" s="11"/>
+      <c r="L75" s="9"/>
       <c r="M75" s="3">
         <f t="shared" ref="M75:M82" si="54">E75</f>
         <v>723</v>
@@ -3892,8 +3885,8 @@
       </c>
       <c r="I76" s="3"/>
       <c r="J76" s="3"/>
-      <c r="K76" s="7"/>
-      <c r="L76" s="11"/>
+      <c r="K76"/>
+      <c r="L76" s="9"/>
       <c r="M76" s="3">
         <f t="shared" si="54"/>
         <v>1913</v>
@@ -3930,8 +3923,7 @@
       </c>
       <c r="I77" s="3"/>
       <c r="J77" s="3"/>
-      <c r="K77" s="7"/>
-      <c r="L77" s="11"/>
+      <c r="L77" s="9"/>
       <c r="M77" s="3">
         <f t="shared" si="54"/>
         <v>563</v>
@@ -3968,8 +3960,7 @@
       </c>
       <c r="I78" s="3"/>
       <c r="J78" s="3"/>
-      <c r="K78" s="7"/>
-      <c r="L78" s="11"/>
+      <c r="L78" s="9"/>
       <c r="M78" s="3">
         <f t="shared" si="54"/>
         <v>3614</v>
@@ -4006,8 +3997,7 @@
       </c>
       <c r="I79" s="3"/>
       <c r="J79" s="3"/>
-      <c r="K79" s="7"/>
-      <c r="L79" s="11"/>
+      <c r="L79" s="9"/>
       <c r="M79" s="3">
         <f t="shared" si="54"/>
         <v>1292</v>
@@ -4044,8 +4034,7 @@
       </c>
       <c r="I80" s="3"/>
       <c r="J80" s="3"/>
-      <c r="K80" s="7"/>
-      <c r="L80" s="11"/>
+      <c r="L80" s="9"/>
       <c r="M80" s="3">
         <f t="shared" si="54"/>
         <v>979</v>
@@ -4082,8 +4071,7 @@
       </c>
       <c r="I81" s="3"/>
       <c r="J81" s="3"/>
-      <c r="K81" s="7"/>
-      <c r="L81" s="11"/>
+      <c r="L81" s="9"/>
       <c r="M81" s="3">
         <f t="shared" si="54"/>
         <v>136</v>
@@ -4120,8 +4108,7 @@
       </c>
       <c r="I82" s="3"/>
       <c r="J82" s="3"/>
-      <c r="K82" s="7"/>
-      <c r="L82" s="11"/>
+      <c r="L82" s="9"/>
       <c r="M82" s="3">
         <f t="shared" si="54"/>
         <v>1085</v>
@@ -4168,8 +4155,8 @@
         <v>0</v>
       </c>
       <c r="J83" s="4"/>
-      <c r="K83" s="6"/>
-      <c r="L83" s="9"/>
+      <c r="K83" s="3"/>
+      <c r="L83" s="7"/>
       <c r="M83" s="4">
         <f>SUM(M74:M82)</f>
         <v>46351</v>
@@ -4180,14 +4167,13 @@
       </c>
     </row>
     <row r="84" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="K84" s="7"/>
-      <c r="L84" s="11"/>
+      <c r="L84" s="9"/>
     </row>
     <row r="85" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A85" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="L85" s="8"/>
+      <c r="L85" s="6"/>
     </row>
     <row r="86" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
@@ -4479,7 +4465,7 @@
       </c>
       <c r="J93" s="4"/>
       <c r="K93" s="4"/>
-      <c r="L93" s="10"/>
+      <c r="L93" s="8"/>
       <c r="M93" s="4">
         <f t="shared" si="62"/>
         <v>38117</v>
@@ -4515,7 +4501,7 @@
       <c r="I94" s="3"/>
       <c r="J94" s="3"/>
       <c r="M94" s="3">
-        <f t="shared" ref="M94:M95" si="63">E94</f>
+        <f t="shared" ref="M94" si="63">E94</f>
         <v>54</v>
       </c>
       <c r="N94" s="3">
@@ -4574,7 +4560,7 @@
       </c>
       <c r="J96" s="4"/>
       <c r="K96" s="4"/>
-      <c r="L96" s="10"/>
+      <c r="L96" s="8"/>
       <c r="M96" s="4">
         <f t="shared" si="65"/>
         <v>8180</v>
@@ -4597,7 +4583,7 @@
       <c r="H97" s="4"/>
       <c r="I97" s="4"/>
       <c r="J97" s="4"/>
-      <c r="L97" s="8"/>
+      <c r="L97" s="6"/>
       <c r="M97" s="4"/>
       <c r="N97" s="4"/>
     </row>
@@ -4855,7 +4841,7 @@
       </c>
       <c r="J104" s="4"/>
       <c r="K104" s="4"/>
-      <c r="L104" s="10"/>
+      <c r="L104" s="8"/>
       <c r="M104" s="4">
         <f t="shared" si="69"/>
         <v>8096</v>
@@ -4903,7 +4889,7 @@
       </c>
       <c r="J105" s="4"/>
       <c r="K105" s="4"/>
-      <c r="L105" s="10"/>
+      <c r="L105" s="8"/>
       <c r="M105" s="4">
         <f t="shared" si="71"/>
         <v>46267</v>
@@ -5014,10 +5000,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5A4ED89-0403-4F67-9A5F-2AAFDE394116}">
-  <dimension ref="B2:C6"/>
+  <dimension ref="B2:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5065,6 +5051,30 @@
         <v>123</v>
       </c>
     </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B7" t="s">
+        <v>133</v>
+      </c>
+      <c r="C7" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B8" t="s">
+        <v>146</v>
+      </c>
+      <c r="C8" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B9" t="s">
+        <v>146</v>
+      </c>
+      <c r="C9" t="s">
+        <v>148</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>